<commit_message>
Set ARpUIiRC value for renewables to zero
</commit_message>
<xml_diff>
--- a/InputData/elec/ARpUIiRC/Ann Ret per Unit Inc in Relative Cost.xlsx
+++ b/InputData/elec/ARpUIiRC/Ann Ret per Unit Inc in Relative Cost.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\elec\ARpUIiRC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F72A4D27-31B9-46EA-9276-94DDCD36B977}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5816E75E-9918-4142-B974-3CD66F692743}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -13565,15 +13565,6 @@
     <row r="2841" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="B2598:AG2598"/>
-    <mergeCell ref="B2719:AG2719"/>
-    <mergeCell ref="B2837:AG2837"/>
-    <mergeCell ref="B1945:AG1945"/>
-    <mergeCell ref="B2031:AG2031"/>
-    <mergeCell ref="B2153:AG2153"/>
-    <mergeCell ref="B2317:AG2317"/>
-    <mergeCell ref="B2419:AG2419"/>
-    <mergeCell ref="B2509:AG2509"/>
     <mergeCell ref="B1698:AG1698"/>
     <mergeCell ref="B87:AG87"/>
     <mergeCell ref="B112:AG112"/>
@@ -13586,6 +13577,15 @@
     <mergeCell ref="B1390:AG1390"/>
     <mergeCell ref="B1502:AG1502"/>
     <mergeCell ref="B1604:AG1604"/>
+    <mergeCell ref="B2598:AG2598"/>
+    <mergeCell ref="B2719:AG2719"/>
+    <mergeCell ref="B2837:AG2837"/>
+    <mergeCell ref="B1945:AG1945"/>
+    <mergeCell ref="B2031:AG2031"/>
+    <mergeCell ref="B2153:AG2153"/>
+    <mergeCell ref="B2317:AG2317"/>
+    <mergeCell ref="B2419:AG2419"/>
+    <mergeCell ref="B2509:AG2509"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -24996,8 +24996,8 @@
   </sheetPr>
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -25051,8 +25051,7 @@
         <v>47</v>
       </c>
       <c r="B6" s="4">
-        <f>$B$2*Weighting!B107</f>
-        <v>3028.7818497951525</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
@@ -25060,8 +25059,7 @@
         <v>27</v>
       </c>
       <c r="B7" s="4">
-        <f>$B$2*Weighting!B108</f>
-        <v>3865.5382849918251</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
@@ -25121,8 +25119,7 @@
         <v>48</v>
       </c>
       <c r="B14" s="4">
-        <f>$B$2*Weighting!B115</f>
-        <v>5256.8659353766534</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>